<commit_message>
Added multiple test cases
</commit_message>
<xml_diff>
--- a/automation.components/utilities/testDataFile.xlsx
+++ b/automation.components/utilities/testDataFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88473575ac6b2b4b/Desktop/Automation Frameworks/PlayWright Workouts/stable/Playwright-Workout/Training/ExcelDataModel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rames\Desktop\Automation Repository\Playwright.Demoqa.WebApp\stable\Playwright.Demoqa.WebApp\automation.components\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC1048B4C11F46D25BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06FDBD7B-303C-40B7-A727-1B2702AC7EAB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A43FF0-B640-4F7B-BD85-241837A4F11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,10 +200,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,7 +468,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added multisheet pick capability
</commit_message>
<xml_diff>
--- a/automation.components/utilities/testDataFile.xlsx
+++ b/automation.components/utilities/testDataFile.xlsx
@@ -5,15 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88473575ac6b2b4b/Desktop/Automation Frameworks/PlayWright Workouts/stable/Playwright-Workout/Training/ExcelDataModel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rames\Desktop\Automation Repository\Playwright.Demoqa.WebApp\Dev\Playwright.Demoqa.WebApp\automation.components\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC1048B4C11F46D25BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06FDBD7B-303C-40B7-A727-1B2702AC7EAB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0DACC4-7D5C-4D0C-B7C6-439147C252A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Elements-TextBox" sheetId="1" r:id="rId1"/>
+    <sheet name="ElementsPage" sheetId="1" r:id="rId1"/>
+    <sheet name="FormsPage" sheetId="2" r:id="rId2"/>
+    <sheet name="AlertsFramesWindowsPage" sheetId="3" r:id="rId3"/>
+    <sheet name="WidgetsPage" sheetId="4" r:id="rId4"/>
+    <sheet name="InteractionsPage" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="25">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -200,10 +204,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,7 +472,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E3" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,4 +579,312 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8C79A2-B3F3-4B9D-B99D-CB3AE76F78FD}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{082B92AE-3B8B-4562-907F-90111A122438}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{02AACF7E-A0EB-4F69-B1ED-23E82CA3628F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A799F39-1A4C-40DB-B461-239808857802}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{F33341ED-4DCF-4F47-8BD6-830CDC0C48DC}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{C4EA76C2-868A-492D-B340-801FAF96242B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B85457-A271-494A-8705-A4C4E8548E08}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5DCAB596-0F28-4672-9862-D69F02D354A6}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{6DEB6350-DA27-49DF-BEC4-A5324A479A81}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225ABBC4-FD1D-420D-B9A7-642B892575E7}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{D2F4559B-940D-422B-A065-2FB3A071E947}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{DB87010A-705D-4DC8-8E75-7ADD601FD3EE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
trying to add driver method
</commit_message>
<xml_diff>
--- a/automation.components/utilities/testDataFile.xlsx
+++ b/automation.components/utilities/testDataFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rames\Desktop\Automation Repository\Playwright.Demoqa.WebApp\Dev\Playwright.Demoqa.WebApp\automation.components\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D9EB1F-36BD-4CF1-B171-9B01264AD5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F771F5B1-DCB6-45AD-B141-D3988E1767D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="40">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -122,33 +122,21 @@
     <t>Scenario Description</t>
   </si>
   <si>
-    <t>Sce_001</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Completed</t>
-  </si>
-  <si>
     <t>Create_form</t>
   </si>
   <si>
     <t>Create new Enrollment Form</t>
   </si>
   <si>
-    <t>Sce_002</t>
-  </si>
-  <si>
     <t>Edit_form</t>
   </si>
   <si>
     <t>Edit new Enrollment Form</t>
   </si>
   <si>
-    <t>Sce_003</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -156,9 +144,6 @@
   </si>
   <si>
     <t>Update new Enrollment Form</t>
-  </si>
-  <si>
-    <t>Sce_004</t>
   </si>
   <si>
     <t>Addnewrow_form</t>
@@ -255,7 +240,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -540,7 +525,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,66 +555,69 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>